<commit_message>
Bug fixes and new test
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevExternal\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ValidateFormulas" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="Cells_B2B3">ValidateFormulas!$B$2:$B$3</definedName>
     <definedName name="Name">Sheet1!$C$1</definedName>
     <definedName name="NameName">Name+Sheet1!$D$5</definedName>
   </definedNames>
@@ -28,9 +30,113 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>SingelCell</t>
+  </si>
+  <si>
+    <t>MultiCell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>MultiCell incl Text</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Name other sheet</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>CountA</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>AverageA</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Array incl text</t>
+  </si>
+  <si>
+    <t>Name Error</t>
+  </si>
+  <si>
+    <t>Div/0</t>
+  </si>
+  <si>
+    <t>Subtotal(1</t>
+  </si>
+  <si>
+    <t>Subtotal(2</t>
+  </si>
+  <si>
+    <t>Subtotal(3</t>
+  </si>
+  <si>
+    <t>Subtotal(4</t>
+  </si>
+  <si>
+    <t>Subtotal(5</t>
+  </si>
+  <si>
+    <t>Subtotal(6</t>
+  </si>
+  <si>
+    <t>Subtotal(7</t>
+  </si>
+  <si>
+    <t>Subtotal(8</t>
+  </si>
+  <si>
+    <t>Subtotal(9</t>
+  </si>
+  <si>
+    <t>Subtotal(10</t>
+  </si>
+  <si>
+    <t>Subtotal(11</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Single Argument</t>
+  </si>
+  <si>
+    <t>Multi Argument</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,13 +144,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -59,8 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -341,10 +463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,9 +553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -490,4 +614,807 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:N27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="e">
+        <f>d</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="e">
+        <f>0/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <f>SUM($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>SUM($B$2:$B$5)</f>
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <f>SUM($B$2:$B$6)</f>
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <f>SUM(Cells_B2B3)</f>
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <f>SUM(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>SUM(1,3,B4:B5)</f>
+        <v>34</v>
+      </c>
+      <c r="H9" t="e">
+        <f>SUM(#REF!:B3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I9">
+        <f>SUM(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J9">
+        <f>SUM({1;2;4;"Text"})</f>
+        <v>7</v>
+      </c>
+      <c r="L9" t="e">
+        <f>SUM(C2)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M9" t="e">
+        <f>SUM(C3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" t="e">
+        <f>SUM(C2:C3)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>COUNT($B$2)</f>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f>COUNT($B$2:$B$5)</f>
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f>COUNT($B$2:$B$6)</f>
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f>COUNT(Cells_B2B3)</f>
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f>COUNT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <f>COUNT(1,3,B4:B5)</f>
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <f>COUNT(#REF!)</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>COUNT(Name)</f>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>COUNT({1;2;4;"Text"})</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>COUNTA($B$2)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>COUNTA($B$2:$B$5)</f>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <f>COUNTA($B$2:$B$6)</f>
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f>COUNTA(Cells_B2B3)</f>
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f>COUNTA(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f>COUNTA(1,3,B4:B5)</f>
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <f>COUNTA(#REF!)</f>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f>COUNTA(Name)</f>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f>COUNTA({1;2;4;"Text"})</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <f>MIN($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <f>MAX($B$2:$B$5)</f>
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <f>MIN($B$2:$B$6)</f>
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f>MAX(Cells_B2B3)</f>
+        <v>7</v>
+      </c>
+      <c r="F12">
+        <f>MAX(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>MIN(1,3,B4:B5)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" t="e">
+        <f>MAX(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I12">
+        <f>MAX(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J12">
+        <f>MAX({1;2;4;"Text"})</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <f>MAX($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <f>MIN($B$2:$B$5)</f>
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <f>MAX($B$2:$B$6)</f>
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <f>MIN(Cells_B2B3)</f>
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f>MIN(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f>MAX(1,3,B4:B5)</f>
+        <v>18</v>
+      </c>
+      <c r="H13" t="e">
+        <f>MIN(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I13">
+        <f>MIN(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J13">
+        <f>MIN({1;2;4;"Text"})</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE($B$2:$B$5)</f>
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f>AVERAGE($B$2:$B$6)</f>
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(Cells_B2B3)</f>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f>AVERAGE(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f>AVERAGE(1,3,B4:B5)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H14" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I14">
+        <f>AVERAGE(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J14">
+        <f>AVERAGE({1;2;4;"Text"})</f>
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>AVERAGEA($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGEA($B$2:$B$5)</f>
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGEA($B$2:$B$6)</f>
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <f>AVERAGEA(Cells_B2B3)</f>
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f>AVERAGEA(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <f>SUM(1,3,B4:B5)</f>
+        <v>34</v>
+      </c>
+      <c r="H15" t="e">
+        <f>AVERAGEA(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I15">
+        <f>AVERAGEA(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J15">
+        <f>AVERAGEA({1;2;4;"Text"})</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f>PRODUCT($B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f>PRODUCT($B$2:$B$5)</f>
+        <v>4536</v>
+      </c>
+      <c r="D16">
+        <f>PRODUCT($B$2:$B$6)</f>
+        <v>4536</v>
+      </c>
+      <c r="E16">
+        <f>PRODUCT(Cells_B2B3)</f>
+        <v>21</v>
+      </c>
+      <c r="F16">
+        <f>PRODUCT(1)</f>
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <f>PRODUCT(1,3,B4:B5)</f>
+        <v>648</v>
+      </c>
+      <c r="H16" t="e">
+        <f>PRODUCT(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I16">
+        <f>PRODUCT(Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J16">
+        <f>PRODUCT({1;2;4;"Text"})</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <f>SUBTOTAL(1,B2)</f>
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <f>SUBTOTAL(1,$B$2:$B$5)</f>
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f>SUBTOTAL(1,$B$2:$B$6)</f>
+        <v>10</v>
+      </c>
+      <c r="E17">
+        <f>SUBTOTAL(1,Cells_B2B3)</f>
+        <v>5</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" t="e">
+        <f>SUBTOTAL(1,#REF!:B3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I17">
+        <f>SUBTOTAL(1,Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <f>SUBTOTAL(2,$B$2)</f>
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>SUBTOTAL(2,$B$2:$B$5)</f>
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f>SUBTOTAL(2,$B$2:$B$6)</f>
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <f>SUBTOTAL(2,Cells_B2B3)</f>
+        <v>2</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" t="e">
+        <f>SUBTOTAL(2,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I18">
+        <f>SUBTOTAL(2,Name)</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <f>SUBTOTAL(3,$B$2)</f>
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <f>SUBTOTAL(3,$B$2:$B$5)</f>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f>SUBTOTAL(3,$B$2:$B$6)</f>
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <f>SUBTOTAL(3,Cells_B2B3)</f>
+        <v>2</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" t="e">
+        <f>SUBTOTAL(3,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I19">
+        <f>SUBTOTAL(3,Name)</f>
+        <v>1</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <f>SUBTOTAL(4,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <f>SUBTOTAL(4,$B$2:$B$5)</f>
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <f>SUBTOTAL(4,$B$2:$B$6)</f>
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <f>SUBTOTAL(4,Cells_B2B3)</f>
+        <v>7</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" t="e">
+        <f>SUBTOTAL(4,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I20">
+        <f>SUBTOTAL(4,Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <f>SUBTOTAL(5,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <f>SUBTOTAL(5,$B$2:$B$5)</f>
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <f>SUBTOTAL(5,$B$2:$B$6)</f>
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <f>SUBTOTAL(5,Cells_B2B3)</f>
+        <v>3</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" t="e">
+        <f>SUBTOTAL(5,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I21">
+        <f>SUBTOTAL(5,Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <f>SUBTOTAL(6,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <f>SUBTOTAL(6,$B$2:$B$5)</f>
+        <v>4536</v>
+      </c>
+      <c r="D22">
+        <f>SUBTOTAL(6,$B$2:$B$6)</f>
+        <v>4536</v>
+      </c>
+      <c r="E22">
+        <f>SUBTOTAL(6,Cells_B2B3)</f>
+        <v>21</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" t="e">
+        <f>SUBTOTAL(6,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I22">
+        <f>SUBTOTAL(6,Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="e">
+        <f>SUBTOTAL(7,$B$2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23">
+        <f>SUBTOTAL(7,$B$2:$B$5)</f>
+        <v>6.4807406984078604</v>
+      </c>
+      <c r="D23">
+        <f>SUBTOTAL(7,$B$2:$B$6)</f>
+        <v>6.4807406984078604</v>
+      </c>
+      <c r="E23">
+        <f>SUBTOTAL(7,Cells_B2B3)</f>
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" t="e">
+        <f>SUBTOTAL(7,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I23" t="e">
+        <f>SUBTOTAL(7,Name)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <f>SUBTOTAL(8,$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <f>SUBTOTAL(8,$B$2:$B$5)</f>
+        <v>5.6124860801609122</v>
+      </c>
+      <c r="D24">
+        <f>SUBTOTAL(8,$B$2:$B$6)</f>
+        <v>5.6124860801609122</v>
+      </c>
+      <c r="E24">
+        <f>SUBTOTAL(8,Cells_B2B3)</f>
+        <v>2</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" t="e">
+        <f>SUBTOTAL(8,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I24">
+        <f>SUBTOTAL(8,Name)</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25">
+        <f>SUBTOTAL(9,$B$2)</f>
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <f>SUBTOTAL(9,$B$2:$B$5)</f>
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <f>SUBTOTAL(9,$B$2:$B$6)</f>
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <f>SUBTOTAL(9,Cells_B2B3)</f>
+        <v>10</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" t="e">
+        <f>SUBTOTAL(9,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I25">
+        <f>SUBTOTAL(9,Name)</f>
+        <v>130</v>
+      </c>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="e">
+        <f>SUBTOTAL(10,$B$2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C26">
+        <f>SUBTOTAL(10,$B$2:$B$5)</f>
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <f>SUBTOTAL(10,$B$2:$B$6)</f>
+        <v>42</v>
+      </c>
+      <c r="E26">
+        <f>SUBTOTAL(10,Cells_B2B3)</f>
+        <v>8</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" t="e">
+        <f>SUBTOTAL(10,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I26" t="e">
+        <f>SUBTOTAL(10,Name)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <f>SUBTOTAL(11,$B$2)</f>
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>SUBTOTAL(11,$B$2:$B$5)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D27">
+        <f>SUBTOTAL(11,$B$2:$B$6)</f>
+        <v>31.5</v>
+      </c>
+      <c r="E27">
+        <f>SUBTOTAL(11,Cells_B2B3)</f>
+        <v>4</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" t="e">
+        <f>SUBTOTAL(11,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I27">
+        <f>SUBTOTAL(11,Name)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Text function. Fixed bug setting uri's to lower case on save.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -708,7 +708,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -744,6 +744,10 @@
       <c r="D1">
         <f>A2+-1</f>
         <v>15</v>
+      </c>
+      <c r="F1" t="str">
+        <f>TEXT(I3,"# ##0,00") &amp; " - " &amp; TEXT(C1,"?/???")</f>
+        <v>349 578 723 238,40 - -9991/554</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1761,7 +1765,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed bug in dependencey chains. Fixed a few Excel functions bugs. Some work on propagating the correct Excel errors between operators. String compareing should not be case sensitive.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/FormulaTest.xlsx
+++ b/EPPlusTest/Workbooks/FormulaTest.xlsx
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Cells_B2B3">ValidateFormulas!$B$2:$B$3</definedName>
+    <definedName name="Cells_B2B3">ValidateFormulas!$B$3:$B$4</definedName>
     <definedName name="Name">Sheet1!$C$1</definedName>
     <definedName name="Name_G5">Sheet3!$G$5</definedName>
     <definedName name="NameName">Name+Sheet1!$D$5</definedName>
@@ -555,9 +555,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -708,10 +706,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,1045 +732,1051 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1">
+        <f>3363482527/400000000*50000000</f>
+        <v>420435315.875</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1">
-        <f>((L3-I3)/I3)/P3</f>
+      <c r="C2">
+        <f>((L4-I4)/I4)/P4</f>
         <v>-18.034296710838554</v>
       </c>
-      <c r="D1">
-        <f>A2+-1</f>
+      <c r="D2">
+        <f>A3+-1</f>
         <v>15</v>
       </c>
-      <c r="F1" t="str">
-        <f>TEXT(I3,"# ##0,00") &amp; " - " &amp; TEXT(C1,"?/???")</f>
+      <c r="F2" t="str">
+        <f>TEXT(I4,"# ##0,00") &amp; " - " &amp; TEXT(C2,"?/???")</f>
         <v>349 578 723 238,40 - -9991/554</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <f>Sheet2!A1+B9+Sheet2!A9+J9</f>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>Sheet2!A1+B10+Sheet2!A9+J10</f>
         <v>16</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="e">
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="e">
         <f>d</f>
         <v>#NAME?</v>
       </c>
-      <c r="D2">
-        <f>A2*-1</f>
+      <c r="D3">
+        <f>A3*-1</f>
         <v>-16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="C3" t="e">
+      <c r="C4" t="e">
         <f>0/0</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D3">
-        <f>D1*1</f>
+      <c r="D4">
+        <f>D2*1</f>
         <v>15</v>
       </c>
-      <c r="I3">
+      <c r="I4">
         <v>349578723238.39771</v>
       </c>
-      <c r="L3">
+      <c r="L4">
         <v>409371020621.32922</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P4" s="3">
         <v>-9.4842073007525979E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="b">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9">
-        <f>SUM($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <f>SUM($B$2:$B$5)</f>
+      <c r="B10">
+        <f>SUM($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <f>SUM($B$3:$B$6)</f>
         <v>40</v>
       </c>
-      <c r="D9">
-        <f>SUM($B$2:$B$6)</f>
+      <c r="D10">
+        <f>SUM($B$3:$B$7)</f>
         <v>40</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f>SUM(Cells_B2B3)</f>
         <v>10</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <f>SUM(1)</f>
         <v>1</v>
       </c>
-      <c r="G9">
-        <f>SUM(1,3,B4:B5)</f>
+      <c r="G10">
+        <f>SUM(1,3,B5:B6)</f>
         <v>34</v>
       </c>
-      <c r="H9" t="e">
-        <f>SUM(#REF!:B3)</f>
+      <c r="H10" t="e">
+        <f>SUM(#REF!:B4)</f>
         <v>#REF!</v>
       </c>
-      <c r="I9">
+      <c r="I10">
         <f>SUM(Name)</f>
         <v>130</v>
       </c>
-      <c r="J9">
+      <c r="J10">
         <f>SUM({1;2;4;"Text";TRUE})</f>
         <v>7</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
         <v>2129121.3509751195</v>
       </c>
-      <c r="L9">
-        <f>SUM(4:5)</f>
+      <c r="L10">
+        <f>SUM(5:6)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
-        <f>COUNT($B$2)</f>
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <f>COUNT($B$2:$B$5)</f>
+      <c r="B11">
+        <f>COUNT($B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f>COUNT($B$3:$B$6)</f>
         <v>4</v>
       </c>
-      <c r="D10">
-        <f>COUNT($B$2:$B$6)</f>
+      <c r="D11">
+        <f>COUNT($B$3:$B$7)</f>
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f>COUNT(Cells_B2B3)</f>
         <v>2</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <f>COUNT(1)</f>
         <v>1</v>
       </c>
-      <c r="G10">
-        <f>COUNT(1,3,B4:B5)</f>
+      <c r="G11">
+        <f>COUNT(1,3,B5:B6)</f>
         <v>4</v>
       </c>
-      <c r="H10">
+      <c r="H11">
         <f>COUNT(#REF!)</f>
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="I11">
         <f>COUNT(Name)</f>
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="J11">
         <f>COUNT({1;2;4;"Text";TRUE})</f>
         <v>3</v>
       </c>
-      <c r="K10">
+      <c r="K11">
         <f>COUNT(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
         <v>65.225975119502039</v>
       </c>
-      <c r="L10">
-        <f>SUM(5:6)</f>
+      <c r="L11">
+        <f>SUM(6:7)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
-        <f>COUNTA($B$2)</f>
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <f>COUNTA($B$2:$B$5)</f>
+      <c r="B12">
+        <f>COUNTA($B$3)</f>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>COUNTA($B$3:$B$6)</f>
         <v>4</v>
       </c>
-      <c r="D11">
-        <f>COUNTA($B$2:$B$6)</f>
+      <c r="D12">
+        <f>COUNTA($B$3:$B$7)</f>
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <f>COUNTA(Cells_B2B3)</f>
         <v>2</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <f>COUNTA(1)</f>
         <v>1</v>
       </c>
-      <c r="G11">
-        <f>COUNTA(1,3,B4:B5)</f>
+      <c r="G12">
+        <f>COUNTA(1,3,B5:B6)</f>
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <f>COUNTA(#REF!)</f>
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <f>COUNTA(Name)</f>
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <f>COUNTA({1;2;4;"Text";TRUE})</f>
         <v>5</v>
       </c>
-      <c r="K11">
+      <c r="K12">
         <f>COUNTA(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
         <v>65.225975119502039</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12">
-        <f>MIN($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <f>MAX($B$2:$B$5)</f>
+      <c r="B13">
+        <f>MIN($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <f>MAX($B$3:$B$6)</f>
         <v>18</v>
       </c>
-      <c r="D12">
-        <f>MIN($B$2:$B$6)</f>
-        <v>3</v>
-      </c>
-      <c r="E12">
+      <c r="D13">
+        <f>MIN($B$3:$B$7)</f>
+        <v>3</v>
+      </c>
+      <c r="E13">
         <f>MAX(Cells_B2B3)</f>
         <v>7</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <f>MAX(1)</f>
         <v>1</v>
       </c>
-      <c r="G12">
-        <f>MIN(1,3,B4:B5)</f>
-        <v>1</v>
-      </c>
-      <c r="H12" t="e">
+      <c r="G13">
+        <f>MIN(1,3,B5:B6)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" t="e">
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I12">
+      <c r="I13">
         <f>MAX(Name)</f>
         <v>130</v>
       </c>
-      <c r="J12">
+      <c r="J13">
         <f>MAX({1;2;4;"Text";TRUE})</f>
         <v>4</v>
       </c>
-      <c r="K12">
+      <c r="K13">
         <f>SUM(Sheet3!E29,Table1[FormulaToSum])+Table1[[#Totals],[Column1]]+Table1[[#Totals],[Decimal ]]</f>
         <v>2129121.3509751195</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13">
-        <f>MAX($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <f>MIN($B$2:$B$5)</f>
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <f>MAX($B$2:$B$6)</f>
+      <c r="B14">
+        <f>MAX($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>MIN($B$3:$B$6)</f>
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <f>MAX($B$3:$B$7)</f>
         <v>18</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f>MIN(Cells_B2B3)</f>
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <f>MIN(1)</f>
         <v>1</v>
       </c>
-      <c r="G13">
-        <f>MAX(1,3,B4:B5)</f>
+      <c r="G14">
+        <f>MAX(1,3,B5:B6)</f>
         <v>18</v>
       </c>
-      <c r="H13" t="e">
+      <c r="H14" t="e">
         <f>MIN(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <f>MIN(Name)</f>
         <v>130</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <f>MIN({1;2;4;"Text";TRUE})</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
-        <f>AVERAGE($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <f>AVERAGE($B$2:$B$5)</f>
+      <c r="B15">
+        <f>AVERAGE($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE($B$3:$B$6)</f>
         <v>10</v>
       </c>
-      <c r="D14">
-        <f>AVERAGE($B$2:$B$6)</f>
+      <c r="D15">
+        <f>AVERAGE($B$3:$B$7)</f>
         <v>10</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f>AVERAGE(Cells_B2B3)</f>
         <v>5</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f>AVERAGE(1)</f>
         <v>1</v>
       </c>
-      <c r="G14">
-        <f>AVERAGE(1,3,B4:B5)</f>
+      <c r="G15">
+        <f>AVERAGE(1,3,B5:B6)</f>
         <v>8.5</v>
       </c>
-      <c r="H14" t="e">
+      <c r="H15" t="e">
         <f>AVERAGE(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <f>AVERAGE(Name)</f>
         <v>130</v>
       </c>
-      <c r="J14">
+      <c r="J15">
         <f>AVERAGE({1;2;4;"Text";TRUE})</f>
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <f>AVERAGEA($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <f>AVERAGEA($B$2:$B$5)</f>
+      <c r="B16">
+        <f>AVERAGEA($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <f>AVERAGEA($B$3:$B$6)</f>
         <v>10</v>
       </c>
-      <c r="D15">
-        <f>AVERAGEA($B$2:$B$6)</f>
+      <c r="D16">
+        <f>AVERAGEA($B$3:$B$7)</f>
         <v>8</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <f>AVERAGEA(Cells_B2B3)</f>
         <v>5</v>
       </c>
-      <c r="F15">
+      <c r="F16">
         <f>AVERAGEA(1)</f>
         <v>1</v>
       </c>
-      <c r="G15">
-        <f>SUM(1,3,B4:B5)</f>
+      <c r="G16">
+        <f>SUM(1,3,B5:B6)</f>
         <v>34</v>
       </c>
-      <c r="H15" t="e">
+      <c r="H16" t="e">
         <f>AVERAGEA(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I15">
+      <c r="I16">
         <f>AVERAGEA(Name)</f>
         <v>130</v>
       </c>
-      <c r="J15">
+      <c r="J16">
         <f>AVERAGEA({1;2;4;"Text";TRUE})</f>
         <v>1.75</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <f>PRODUCT($B$2)</f>
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <f>PRODUCT($B$2:$B$5)</f>
+      <c r="B17">
+        <f>PRODUCT($B$3)</f>
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <f>PRODUCT($B$3:$B$6)</f>
         <v>4536</v>
       </c>
-      <c r="D16">
-        <f>PRODUCT($B$2:$B$6)</f>
+      <c r="D17">
+        <f>PRODUCT($B$3:$B$7)</f>
         <v>4536</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <f>PRODUCT(Cells_B2B3)</f>
         <v>21</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <f>PRODUCT(1)</f>
         <v>1</v>
       </c>
-      <c r="G16">
-        <f>PRODUCT(1,3,B4:B5)</f>
+      <c r="G17">
+        <f>PRODUCT(1,3,B5:B6)</f>
         <v>648</v>
       </c>
-      <c r="H16" t="e">
+      <c r="H17" t="e">
         <f>PRODUCT(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I16">
+      <c r="I17">
         <f>PRODUCT(Name)</f>
         <v>130</v>
       </c>
-      <c r="J16">
+      <c r="J17">
         <f>PRODUCT({1;2;4;"Text";TRUE})</f>
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17">
-        <f>SUBTOTAL(1,B2)</f>
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <f>SUBTOTAL(1,$B$2:$B$5)</f>
+      <c r="B18">
+        <f>SUBTOTAL(1,B3)</f>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <f>SUBTOTAL(1,$B$3:$B$6)</f>
         <v>10</v>
       </c>
-      <c r="D17">
-        <f>SUBTOTAL(1,$B$2:$B$6)</f>
+      <c r="D18">
+        <f>SUBTOTAL(1,$B$3:$B$7)</f>
         <v>10</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <f>SUBTOTAL(1,Cells_B2B3)</f>
         <v>5</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" t="e">
-        <f>SUBTOTAL(1,#REF!:B3)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I17">
-        <f>SUBTOTAL(1,Name)</f>
-        <v>130</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <f>SUBTOTAL(2,$B$2)</f>
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <f>SUBTOTAL(2,$B$2:$B$5)</f>
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <f>SUBTOTAL(2,$B$2:$B$6)</f>
-        <v>4</v>
-      </c>
-      <c r="E18">
-        <f>SUBTOTAL(2,Cells_B2B3)</f>
-        <v>2</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" t="e">
-        <f>SUBTOTAL(2,#REF!)</f>
+        <f>SUBTOTAL(1,#REF!:B4)</f>
         <v>#REF!</v>
       </c>
       <c r="I18">
-        <f>SUBTOTAL(2,Name)</f>
-        <v>1</v>
+        <f>SUBTOTAL(1,Name)</f>
+        <v>130</v>
       </c>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <f>SUBTOTAL(3,$B$2)</f>
+        <f>SUBTOTAL(2,$B$3)</f>
         <v>1</v>
       </c>
       <c r="C19">
-        <f>SUBTOTAL(3,$B$2:$B$5)</f>
+        <f>SUBTOTAL(2,$B$3:$B$6)</f>
         <v>4</v>
       </c>
       <c r="D19">
-        <f>SUBTOTAL(3,$B$2:$B$6)</f>
-        <v>5</v>
+        <f>SUBTOTAL(2,$B$3:$B$7)</f>
+        <v>4</v>
       </c>
       <c r="E19">
-        <f>SUBTOTAL(3,Cells_B2B3)</f>
+        <f>SUBTOTAL(2,Cells_B2B3)</f>
         <v>2</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" t="e">
-        <f>SUBTOTAL(3,#REF!)</f>
+        <f>SUBTOTAL(2,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="I19">
-        <f>SUBTOTAL(3,Name)</f>
+        <f>SUBTOTAL(2,Name)</f>
         <v>1</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <f>SUBTOTAL(4,$B$2)</f>
-        <v>3</v>
+        <f>SUBTOTAL(3,$B$3)</f>
+        <v>1</v>
       </c>
       <c r="C20">
-        <f>SUBTOTAL(4,$B$2:$B$5)</f>
-        <v>18</v>
+        <f>SUBTOTAL(3,$B$3:$B$6)</f>
+        <v>4</v>
       </c>
       <c r="D20">
-        <f>SUBTOTAL(4,$B$2:$B$6)</f>
-        <v>18</v>
+        <f>SUBTOTAL(3,$B$3:$B$7)</f>
+        <v>5</v>
       </c>
       <c r="E20">
-        <f>SUBTOTAL(4,Cells_B2B3)</f>
-        <v>7</v>
+        <f>SUBTOTAL(3,Cells_B2B3)</f>
+        <v>2</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" t="e">
-        <f>SUBTOTAL(4,#REF!)</f>
+        <f>SUBTOTAL(3,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="I20">
-        <f>SUBTOTAL(4,Name)</f>
-        <v>130</v>
+        <f>SUBTOTAL(3,Name)</f>
+        <v>1</v>
       </c>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <f>SUBTOTAL(5,$B$2)</f>
+        <f>SUBTOTAL(4,$B$3)</f>
         <v>3</v>
       </c>
       <c r="C21">
-        <f>SUBTOTAL(5,$B$2:$B$5)</f>
-        <v>3</v>
+        <f>SUBTOTAL(4,$B$3:$B$6)</f>
+        <v>18</v>
       </c>
       <c r="D21">
-        <f>SUBTOTAL(5,$B$2:$B$6)</f>
-        <v>3</v>
+        <f>SUBTOTAL(4,$B$3:$B$7)</f>
+        <v>18</v>
       </c>
       <c r="E21">
-        <f>SUBTOTAL(5,Cells_B2B3)</f>
-        <v>3</v>
+        <f>SUBTOTAL(4,Cells_B2B3)</f>
+        <v>7</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" t="e">
-        <f>SUBTOTAL(5,#REF!)</f>
+        <f>SUBTOTAL(4,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="I21">
-        <f>SUBTOTAL(5,Name)</f>
+        <f>SUBTOTAL(4,Name)</f>
         <v>130</v>
       </c>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <f>SUBTOTAL(6,$B$2)</f>
+        <f>SUBTOTAL(5,$B$3)</f>
         <v>3</v>
       </c>
       <c r="C22">
-        <f>SUBTOTAL(6,$B$2:$B$5)</f>
-        <v>4536</v>
+        <f>SUBTOTAL(5,$B$3:$B$6)</f>
+        <v>3</v>
       </c>
       <c r="D22">
-        <f>SUBTOTAL(6,$B$2:$B$6)</f>
-        <v>4536</v>
+        <f>SUBTOTAL(5,$B$3:$B$7)</f>
+        <v>3</v>
       </c>
       <c r="E22">
-        <f>SUBTOTAL(6,Cells_B2B3)</f>
-        <v>21</v>
+        <f>SUBTOTAL(5,Cells_B2B3)</f>
+        <v>3</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" t="e">
-        <f>SUBTOTAL(6,#REF!)</f>
+        <f>SUBTOTAL(5,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="I22">
-        <f>SUBTOTAL(6,Name)</f>
+        <f>SUBTOTAL(5,Name)</f>
         <v>130</v>
       </c>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="e">
-        <f>SUBTOTAL(7,$B$2)</f>
-        <v>#DIV/0!</v>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>SUBTOTAL(6,$B$3)</f>
+        <v>3</v>
       </c>
       <c r="C23">
-        <f>SUBTOTAL(7,$B$2:$B$5)</f>
-        <v>6.4807406984078604</v>
+        <f>SUBTOTAL(6,$B$3:$B$6)</f>
+        <v>4536</v>
       </c>
       <c r="D23">
-        <f>SUBTOTAL(7,$B$2:$B$6)</f>
-        <v>6.4807406984078604</v>
+        <f>SUBTOTAL(6,$B$3:$B$7)</f>
+        <v>4536</v>
       </c>
       <c r="E23">
-        <f>SUBTOTAL(7,Cells_B2B3)</f>
-        <v>2.8284271247461903</v>
+        <f>SUBTOTAL(6,Cells_B2B3)</f>
+        <v>21</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" t="e">
-        <f>SUBTOTAL(7,#REF!)</f>
+        <f>SUBTOTAL(6,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I23" t="e">
-        <f>SUBTOTAL(7,Name)</f>
-        <v>#DIV/0!</v>
+      <c r="I23">
+        <f>SUBTOTAL(6,Name)</f>
+        <v>130</v>
       </c>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <f>SUBTOTAL(8,$B$2)</f>
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="B24" t="e">
+        <f>SUBTOTAL(7,$B$3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C24">
-        <f>SUBTOTAL(8,$B$2:$B$5)</f>
-        <v>5.6124860801609122</v>
+        <f>SUBTOTAL(7,$B$3:$B$6)</f>
+        <v>6.4807406984078604</v>
       </c>
       <c r="D24">
-        <f>SUBTOTAL(8,$B$2:$B$6)</f>
-        <v>5.6124860801609122</v>
+        <f>SUBTOTAL(7,$B$3:$B$7)</f>
+        <v>6.4807406984078604</v>
       </c>
       <c r="E24">
-        <f>SUBTOTAL(8,Cells_B2B3)</f>
-        <v>2</v>
+        <f>SUBTOTAL(7,Cells_B2B3)</f>
+        <v>2.8284271247461903</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" t="e">
-        <f>SUBTOTAL(8,#REF!)</f>
+        <f>SUBTOTAL(7,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I24">
-        <f>SUBTOTAL(8,Name)</f>
-        <v>0</v>
+      <c r="I24" t="e">
+        <f>SUBTOTAL(7,Name)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <f>SUBTOTAL(9,$B$2)</f>
-        <v>3</v>
+        <f>SUBTOTAL(8,$B$3)</f>
+        <v>0</v>
       </c>
       <c r="C25">
-        <f>SUBTOTAL(9,$B$2:$B$5)</f>
-        <v>40</v>
+        <f>SUBTOTAL(8,$B$3:$B$6)</f>
+        <v>5.6124860801609122</v>
       </c>
       <c r="D25">
-        <f>SUBTOTAL(9,$B$2:$B$6)</f>
-        <v>40</v>
+        <f>SUBTOTAL(8,$B$3:$B$7)</f>
+        <v>5.6124860801609122</v>
       </c>
       <c r="E25">
-        <f>SUBTOTAL(9,Cells_B2B3)</f>
-        <v>10</v>
+        <f>SUBTOTAL(8,Cells_B2B3)</f>
+        <v>2</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" t="e">
-        <f>SUBTOTAL(9,#REF!)</f>
+        <f>SUBTOTAL(8,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="I25">
-        <f>SUBTOTAL(9,Name)</f>
-        <v>130</v>
+        <f>SUBTOTAL(8,Name)</f>
+        <v>0</v>
       </c>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="e">
-        <f>SUBTOTAL(10,$B$2)</f>
-        <v>#DIV/0!</v>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f>SUBTOTAL(9,$B$3)</f>
+        <v>3</v>
       </c>
       <c r="C26">
-        <f>SUBTOTAL(10,$B$2:$B$5)</f>
-        <v>42</v>
+        <f>SUBTOTAL(9,$B$3:$B$6)</f>
+        <v>40</v>
       </c>
       <c r="D26">
-        <f>SUBTOTAL(10,$B$2:$B$6)</f>
-        <v>42</v>
+        <f>SUBTOTAL(9,$B$3:$B$7)</f>
+        <v>40</v>
       </c>
       <c r="E26">
-        <f>SUBTOTAL(10,Cells_B2B3)</f>
-        <v>8</v>
+        <f>SUBTOTAL(9,Cells_B2B3)</f>
+        <v>10</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" t="e">
-        <f>SUBTOTAL(10,#REF!)</f>
+        <f>SUBTOTAL(9,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I26" t="e">
-        <f>SUBTOTAL(10,Name)</f>
-        <v>#DIV/0!</v>
+      <c r="I26">
+        <f>SUBTOTAL(9,Name)</f>
+        <v>130</v>
       </c>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27">
-        <f>SUBTOTAL(11,$B$2)</f>
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B27" t="e">
+        <f>SUBTOTAL(10,$B$3)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="C27">
-        <f>SUBTOTAL(11,$B$2:$B$5)</f>
-        <v>31.5</v>
+        <f>SUBTOTAL(10,$B$3:$B$6)</f>
+        <v>42</v>
       </c>
       <c r="D27">
-        <f>SUBTOTAL(11,$B$2:$B$6)</f>
-        <v>31.5</v>
+        <f>SUBTOTAL(10,$B$3:$B$7)</f>
+        <v>42</v>
       </c>
       <c r="E27">
-        <f>SUBTOTAL(11,Cells_B2B3)</f>
-        <v>4</v>
+        <f>SUBTOTAL(10,Cells_B2B3)</f>
+        <v>8</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" t="e">
+        <f>SUBTOTAL(10,#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I27" t="e">
+        <f>SUBTOTAL(10,Name)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f>SUBTOTAL(11,$B$3)</f>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>SUBTOTAL(11,$B$3:$B$6)</f>
+        <v>31.5</v>
+      </c>
+      <c r="D28">
+        <f>SUBTOTAL(11,$B$3:$B$7)</f>
+        <v>31.5</v>
+      </c>
+      <c r="E28">
+        <f>SUBTOTAL(11,Cells_B2B3)</f>
+        <v>4</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" t="e">
         <f>SUBTOTAL(11,#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="I27">
+      <c r="I28">
         <f>SUBTOTAL(11,Name)</f>
         <v>0</v>
       </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="J28" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="e">
-        <f>VLOOKUP("7",B2:B6,1)</f>
+      <c r="B30" t="e">
+        <f>VLOOKUP("7",B3:B7,1)</f>
         <v>#N/A</v>
       </c>
-      <c r="C29" t="e">
-        <f>VLOOKUP(8,B2:B6,FALSE)</f>
+      <c r="C30" t="e">
+        <f>VLOOKUP(8,B3:B7,FALSE)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D29">
-        <f>VLOOKUP(7,B2:B6,1)</f>
+      <c r="D30">
+        <f>VLOOKUP(7,B3:B7,1)</f>
         <v>7</v>
       </c>
-      <c r="E29" t="e">
+      <c r="E30" t="e">
         <f>VLOOKUP(8,{1;2;3;4},1,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <f>VLOOKUP(8,{1;2;3;4;10},1,TRUE)</f>
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B31">
-        <f>IF(B2&gt;3,B3,B5)</f>
+      <c r="B32">
+        <f>IF(B3&gt;3,B4,B6)</f>
         <v>18</v>
       </c>
-      <c r="C31">
-        <f>IF((B2*B3)*C1&lt;0,(B2*B3)*C1,ABS((B2*B3)*C1))</f>
+      <c r="C32">
+        <f>IF((B3*B4)*C2&lt;0,(B3*B4)*C2,ABS((B3*B4)*C2))</f>
         <v>-378.72023092760963</v>
       </c>
-      <c r="D31">
-        <f>IF((B2*B3)*C1&lt;0,ABS((B2*B3)*C1),(B2*B3)*C1)</f>
+      <c r="D32">
+        <f>IF((B3*B4)*C2&lt;0,ABS((B3*B4)*C2),(B3*B4)*C2)</f>
         <v>378.72023092760963</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" t="e">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="e">
         <f>SUM(D:D)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D33" t="b">
-        <f>B4=B3</f>
+      <c r="D34" t="b">
+        <f>B5=B4</f>
         <v>0</v>
       </c>
-      <c r="E33" t="b">
-        <f>C25=D25</f>
-        <v>1</v>
-      </c>
-      <c r="F33" t="e">
-        <f>E38=E39</f>
+      <c r="E34" t="b">
+        <f>C26=D26</f>
+        <v>1</v>
+      </c>
+      <c r="F34" t="e">
+        <f>E39=E40</f>
         <v>#N/A</v>
       </c>
-      <c r="G33" t="b">
-        <f>LEFT(A22,5)=LEFT(A23,5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34">
+      <c r="G34" t="b">
+        <f>LEFT(A23,5)=LEFT(A24,5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35">
         <f>COUNT(D:D)</f>
         <v>24</v>
       </c>
-      <c r="D34" t="b">
-        <f>C30=D30</f>
-        <v>1</v>
-      </c>
-      <c r="E34" t="e">
-        <f>D38=D39</f>
+      <c r="D35" t="b">
+        <f>C31=D31</f>
+        <v>1</v>
+      </c>
+      <c r="E35" t="e">
+        <f>D39=D40</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F34" t="e">
-        <f>G38=H38</f>
+      <c r="F35" t="e">
+        <f>G39=H39</f>
         <v>#NULL!</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="e">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="e">
         <f>d</f>
         <v>#NAME?</v>
       </c>
-      <c r="B38" t="e">
-        <f>SUM(I38)</f>
+      <c r="B39" t="e">
+        <f>SUM(I39)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="C38" t="e">
-        <f>SUM(C2:C3)</f>
+      <c r="C39" t="e">
+        <f>SUM(C3:C4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D38" t="e">
+      <c r="D39" t="e">
         <f>1+"a"</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E38" t="e">
-        <f>VLOOKUP(8,I9:I27,0,FALSE)</f>
+      <c r="E39" t="e">
+        <f>VLOOKUP(8,I10:I28,0,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="F38" t="e">
+      <c r="F39" t="e">
         <f>POWER(100,10000000000000)</f>
         <v>#NUM!</v>
       </c>
-      <c r="G38" t="e">
-        <f>B1 B2</f>
+      <c r="G39" t="e">
+        <f>B2 B3</f>
         <v>#NULL!</v>
       </c>
-      <c r="H38" t="e">
-        <f>SUM(#REF!:B3)</f>
+      <c r="H39" t="e">
+        <f>SUM(#REF!:B4)</f>
         <v>#REF!</v>
       </c>
-      <c r="I38" t="e">
+      <c r="I39" t="e">
         <f>0/0</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="e">
-        <f>SUM(A38)</f>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="e">
+        <f>SUM(A39)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D39" t="e">
-        <f>SUBTOTAL(45,J9:J26)</f>
+      <c r="D40" t="e">
+        <f>SUBTOTAL(45,J10:J27)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E39" t="e">
+      <c r="E40" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="H39" t="e">
+      <c r="H40" t="e">
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="e">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="e">
         <f ca="1">Dp()</f>
         <v>#NAME?</v>
       </c>
-      <c r="D40" t="e">
-        <f>SUMPRODUCT(B2,B3:B4)</f>
+      <c r="D41" t="e">
+        <f>SUMPRODUCT(B3,B4:B5)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H40" t="e">
+      <c r="H41" t="e">
         <f>#REF!:#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="D41" t="e">
-        <f>B1:B2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H41" t="e">
-        <f ca="1">D5()</f>
-        <v>#REF!</v>
-      </c>
-    </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42"/>
+      <c r="D42" t="e">
+        <f>B2:B3</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="H42" t="e">
-        <f ca="1">D5(21)</f>
+        <f ca="1">D6()</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43"/>
+      <c r="H43" t="e">
+        <f ca="1">D6(21)</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A36:I36"/>
-    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="A37:I37"/>
+    <mergeCell ref="D33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>